<commit_message>
Updates from Neil P Nov 12th
</commit_message>
<xml_diff>
--- a/i18n/excel/dk.seges.xlsx
+++ b/i18n/excel/dk.seges.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="418">
   <si>
     <t xml:space="preserve">KEY</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t xml:space="preserve">Μοντέλα SEGES/AU DSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pt</t>
   </si>
   <si>
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.description</t>
@@ -1230,7 +1251,7 @@
 The system also includes models for pest control in cereals.
 The models require information from field registration typically in the period from GS 30-31 to GS 65-71
 (assessments of frequency of plants attacked) and for some diseases also precipitation is required
-(days with more than 1 mm rain). Before getting information on need for treatments – information on crop,
+(days with more than 1 mm rain). Before getting information on need for treatments - information on crop,
 cultivars susceptibility and growth stage (BBCH) is required.
 The growers need to check the crops at weekly intervals or as a minimum follow the risk based on precipitation
 or regional monitoring data for risk evaluation. In the Danish system fungicides and dose rates are
@@ -1246,20 +1267,12 @@
 2. Secher, B.J., Jørgensen, L.N, Murali N.S. &amp; Boll P.S. (1995). Field Validation of a
 Decision Support System for Control of Pests and Diseases in Cereals in Denmark.
 Pesticide Science, 45, 195-199.
-3. Henriksen. K.E.; Jørgensen, L.N. &amp; Nielsen, G.C.(2000) PC-Plant Protection –a tool to
-reduce fungicide input in winter wheat, winter barley and spring barley in Denmark.
+3. Henriksen. K.E.; Jærgensen, L.N. &amp; Nielsen, G.C.(2000) PC-Plant Protection - a tool to reduce fungicide input in winter wheat, winter barley and spring barley in Denmark.
 Brighton Crop Protection Conference. Pest and diseases. 835-840.
-4. Jørgensen, L.N. &amp; Henriksen, K E. (2002) Control of diseases in different winter wheat
-varieties using thresholds and appropriate dosages. Petria vol 12 (1/2) 87-94
-5. Hagelskjær, L.&amp; Jørgensen, LN, 2003 A web-based decision support system for
-integrated management of diesases and pest s in cereals. EPPO Bulletin 33, 467-471.
-6. Jørgensen, LN; Matzen, M, Nielsen, GC, Jalli, M; Ronis; Djule, A; Anderson, B; Ficke, A., Djule, A
-(2020) Validation of risk models for control of leaf blotch diseases in wheat in the Nordic and
-Baltic countries European Journal of Plante Pathology,. https://doi.org/10.1007/si 0658-020-02025-6
-7. Jørgensen, LN; Matzen, N, Heick, T M, Madsen, HP; Kristjansen, H S; Kirkegaard, S;
-Almskou-Dahlgaard, A; Kristoffersen, R (2020). Control strategies in different cultivars.
-Applied Crop Protection 2019.DCA rapport, 167, 58-71.
-https://dcapub.au.dk/djfpublikation/index.asp?action=show&amp;id=1325
+4. Jørgensen, L.N. &amp; Henriksen, K E. (2002) Control of diseases in different winter wheat varieties using thresholds and appropriate dosages. Petria vol 12 (1/2) 87-94
+5. Hagelskjær, L.&amp; Jørgensen, LN, 2003 A web-based decision support system for integrated management of diesases and pest s in cereals. EPPO Bulletin 33, 467-471.
+6. Jørgensen, LN; Matzen, M, Nielsen, GC, Jalli, M; Ronis; Djule, A; Anderson, B; Ficke, A., Djule, A (2020) Validation of risk models for control of leaf blotch diseases in wheat in the Nordic and Baltic countries European Journal of Plante Pathology,. https://doi.org/10.1007/si 0658-020-02025-6
+7. Jørgensen, LN; Matzen, N, Heick, T M, Madsen, HP; Kristjansen, H S; Kirkegaard, S; Almskou-Dahlgaard, A; Kristoffersen, R (2020). Control strategies in different cultivars. Applied Crop Protection 2019.DCA rapport, 167, 58-71. https://dcapub.au.dk/djfpublikation/index.asp?action=show&amp;id=1325
 </t>
   </si>
   <si>
@@ -1305,7 +1318,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.CPO.output.warning_status_interpretation.0.explanation</t>
   </si>
   <si>
-    <t xml:space="preserve">The growers need to check the crops at weekly intervals or as a minimum follow the risk based on precipitation or regional monitoring data for risk evaluation. In the Danish system fungicides and dose rates arerecommended. In the IPM-decision system only a recommendation to treat or not to treat is given.</t>
+    <t xml:space="preserve">The growers need to check the crops at weekly intervals or as a minimum follow the risk based on precipitation or regional monitoring data for risk evaluation. In the Danish system fungicides and dose rates are recommended. In the IPM-decision system only a recommendation to treat or not to treat is given.</t>
   </si>
   <si>
     <t xml:space="preserve">dk.seges.1_1.models.CPO.output.warning_status_interpretation.0.recommended_action</t>
@@ -1377,7 +1390,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1388,6 +1401,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -1432,7 +1451,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1441,12 +1460,24 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1458,6 +1489,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1548,18 +1639,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="107.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="109.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="106.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="10" style="2" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -1587,1340 +1687,1692 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="0" t="s">
+    </row>
+    <row r="2" s="2" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>40</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>85</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>112</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>121</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>130</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>148</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>166</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>184</v>
+      </c>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>190</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="G23" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="B23" s="4" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>225</v>
+      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="I25" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="C26" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>221</v>
-      </c>
       <c r="D26" s="0" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>237</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="I27" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>233</v>
-      </c>
       <c r="D28" s="0" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="I29" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="C30" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>243</v>
-      </c>
       <c r="D30" s="0" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>255</v>
-      </c>
-      <c r="F31" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="G31" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="H31" s="0" t="s">
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="B31" s="4" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>253</v>
-      </c>
       <c r="D32" s="0" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>266</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>276</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>285</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="I35" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="C36" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>281</v>
-      </c>
       <c r="D36" s="0" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>294</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>304</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>310</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>318</v>
+      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="E41" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="F41" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="H41" s="0" t="s">
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+    </row>
+    <row r="41" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="I41" s="0" t="s">
+      <c r="B41" s="4" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>340</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="G43" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="H43" s="0" t="s">
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+    </row>
+    <row r="43" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="I43" s="0" t="s">
+      <c r="B43" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="C43" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="H43" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="G44" s="0" t="s">
+      <c r="I43" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="H44" s="0" t="s">
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="I44" s="0" t="s">
+      <c r="B44" s="4" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="C44" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="D44" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="E44" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="F44" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="G44" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="H44" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="G45" s="0" t="s">
+      <c r="I44" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="H45" s="0" t="s">
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+    </row>
+    <row r="45" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="I45" s="0" t="s">
+      <c r="B45" s="4" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="C45" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="F46" s="0" t="s">
+      <c r="H45" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="I45" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+    </row>
+    <row r="46" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="B46" s="4" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>381</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2938,19 +3390,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="121.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.02"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -2978,270 +3430,424 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="115.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+        <v>391</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
+        <v>394</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>389</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+        <v>396</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+        <v>398</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+        <v>400</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+        <v>401</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+        <v>403</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+        <v>405</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+        <v>407</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+        <v>408</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+        <v>407</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+        <v>410</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+        <v>407</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+        <v>412</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+        <v>407</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+        <v>414</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+        <v>407</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>409</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+        <v>416</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+        <v>417</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Fixed update from Neil P (last commit incorrect)
</commit_message>
<xml_diff>
--- a/i18n/excel/dk.seges.xlsx
+++ b/i18n/excel/dk.seges.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="419">
   <si>
     <t xml:space="preserve">KEY</t>
   </si>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">dk.seges.1_1.name</t>
   </si>
   <si>
-    <t xml:space="preserve">SEGES/AU DSS models</t>
+    <t xml:space="preserve">SEGES DSS models</t>
   </si>
   <si>
     <t xml:space="preserve">SEGES/AU EHS-Modelle</t>
@@ -98,10 +98,10 @@
   <si>
     <t xml:space="preserve">THE PEST: Leaf blotch diseases of wheat can be caused by septoria tritici blotch (Zymoseptoria tritici) and staganospora nodorum blotch (Parastagonospora nodorum), which are both  favoured by wet conditions. 
 THE DECISION: Fungicide treatments may need to be applied between stem extension and ear emergence, mainly to protect the upper leaves.  
-THE MODEL: The humidity model estimates risk of septoria tritici blotch infections in winter wheat. Risk of attack is assumed after 20 hours with continuous wetness. A wet hour is defined as minimum 0,2 mm precipitation in an hour or minimum 85% relative humidity. 
-THE PARAMETERS: Weather data from GS 31 are used. In addition, the dates of occurrence of growth stages 31 and 32 are entered. The model calculates the expected date for the other stages. This can be adjusted manually. Adding information on fungicide spraying dates is vital for the model. After spraying, the model assumes that the crop is protected for 10 days. The thresholds for number of wet hours and relative humidity can be adjusted manually.  
+THE MODEL: Weather data from GS 31 are used. The humidity model estimates risk of septoria tritici blotch infections in winter wheat. Risk of attack is assumed after 20 hours with continuous wetness. A wet hour is defined as minimum 0,2 mm precipitation in an hour or minimum 85% relative humidity. 
+THE PARAMETERS:  Dates of key growth stages are given as default values, but these may not be correct for your location.  To obtain accurate risk predictions it is essential to click on the 'Edit parameters' button, enter the estimated dates of GS31 (first node detectable), GS32 (second node; third upper leaf emerging), GS33 (third node; second upper leaf emerging), GS37/39 (uppermost flag leaf emerging)  and GS75 (grain content milky), then click on the 'Save' button.  These estimated dates can be updated during the season as growth stages are reached. Adding information on septoria fungicide spray dates is vital for the model. This is also done in 'Edit parameters'.  Clicking on 'Save' will keep the spray dates entered.  After spraying, the model assumes that the crop is protected for 10 days.   
 SOURCE: Created by Aahus University and SEGES and released in Denmark in 2017. Tested in Lithuania, Norway, Sweden, Finland and Denmark in 2018 and 2019. 
-ASSUMPTIONS: septoria tritici blotch is present and periods with high humidity create risk for a damaging epidemic
+ASSUMPTIONS: septoria tritici blotch is present in the crop and periods with high humidity create risk for a damaging epidemic
 </t>
   </si>
   <si>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.execution.input_schema.properties.configParameters.properties.dateGs75.title</t>
   </si>
   <si>
-    <t xml:space="preserve">Date of all kernels fully developed (GS75) (YYYY-MM-DD)</t>
+    <t xml:space="preserve">Grain filling (GS75) (YYYY-MM-DD)</t>
   </si>
   <si>
     <t xml:space="preserve">Datum Mitte Milchreife (BBCH 75) (JJJJ-MM-TT)</t>
@@ -688,7 +688,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.chart_groups.G1.title</t>
   </si>
   <si>
-    <t xml:space="preserve">Disease development</t>
+    <t xml:space="preserve">Consecutive humid hours</t>
   </si>
   <si>
     <t xml:space="preserve">Krankheitsentwicklung</t>
@@ -838,33 +838,36 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.result_parameters.HPHPP.description</t>
   </si>
   <si>
+    <t xml:space="preserve">Number of consecutive humid hours, corrected for period of fungicide protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feuchte Periodenstunde (aufeinanderfolgende feuchte Stunden), korrigiert um die Dauer der Schutzwirkung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trajanje obdobja vlažnosti (zaporedne mokre ure), popravljena za obdobje zaščite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vochtig-periode-uur (opeenvolgende vochtige uren) gecorrigeerd voor beschermingsperiode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fugtig periodetime (på hinanden følgende fugtige timer) korrigeret for beskyttelsesperiode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuktig periodtimme (på varandra följande fuktiga timmar) korrigerad för skyddsperiod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ώρα υγρής περιόδου (διαδοχικές υγρές ώρες) διορθωμένη για την περίοδο προστασίας</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuktig periode time (påfølgende fuktige timer) korrigert for beskyttelsesperiode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.result_parameters.HPHPP.title</t>
+  </si>
+  <si>
     <t xml:space="preserve">Humid period hour (consecutive humid hours) corrected for protection period</t>
   </si>
   <si>
-    <t xml:space="preserve">Feuchte Periodenstunde (aufeinanderfolgende feuchte Stunden), korrigiert um die Dauer der Schutzwirkung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trajanje obdobja vlažnosti (zaporedne mokre ure), popravljena za obdobje zaščite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vochtig-periode-uur (opeenvolgende vochtige uren) gecorrigeerd voor beschermingsperiode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fugtig periodetime (på hinanden følgende fugtige timer) korrigeret for beskyttelsesperiode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuktig periodtimme (på varandra följande fuktiga timmar) korrigerad för skyddsperiod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ώρα υγρής περιόδου (διαδοχικές υγρές ώρες) διορθωμένη για την περίοδο προστασίας</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fuktig periode time (påfølgende fuktige timer) korrigert for beskyttelsesperiode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.result_parameters.HPHPP.title</t>
-  </si>
-  <si>
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.result_parameters.SPP.description</t>
   </si>
   <si>
@@ -1051,7 +1054,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.warning_status_interpretation.2.explanation</t>
   </si>
   <si>
-    <t xml:space="preserve">Based on current observations entered and weather data, the risk of septoria is low. This model runs March-June.  Continue to check for risk updates and monitor crops. Update crop growth stage and date of fungicide applications through the season</t>
+    <t xml:space="preserve">Based on weather data and current estimates of crop growth stages and septoria spray dates, the risk of septoria is low. Go to 'Edit parameters' to check and update growth stages and spray dates. This model runs March-June.  </t>
   </si>
   <si>
     <t xml:space="preserve">Auf der Grundlage der eingegebenen aktuellen Beobachtungen und Wetterdaten ist das Risiko von Septoria gering. Dieses Modell läuft von März bis Juni.  Prüfen Sie weiterhin auf Risikoaktualisierungen und überwachen Sie die Kulturen. Aktualisieren Sie das Entwicklungsstadium der Pflanzen und das Datum der Fungizidanwendungen während der Saison.</t>
@@ -1105,7 +1108,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.warning_status_interpretation.3.explanation</t>
   </si>
   <si>
-    <t xml:space="preserve">Based on current observations entered and weather data, the risk of septoria is moderate.</t>
+    <t xml:space="preserve">Based on weather data and current estimates of crop growth stages and septoria spray dates, the risk of septoria is moderate. Go to 'Edit parameters' to check and update growth stages and spray dates. This model runs March-June. </t>
   </si>
   <si>
     <t xml:space="preserve">Auf der Grundlage der aktuell eingegebenen Beobachtungen und Wetterdaten besteht ein mittleres Septoria-Risiko.</t>
@@ -1132,8 +1135,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.warning_status_interpretation.3.recommended_action</t>
   </si>
   <si>
-    <t xml:space="preserve">If the threshold of 20 hours humidity is not  exceeded, but other diseases are assessed to also cause a risk and the crop has not been treated in the last ten days, choose an effective fungicide which also covers  control of septoria. 
-This model runs March-June.  Continue to check for risk updates and monitor crops. Update  crop growth stage and date of fungicide applications through the season</t>
+    <t xml:space="preserve">If the threshold of 20 hours humidity is not exceeded, but other diseases are assessed to also cause a risk and the crop has not been treated in the last ten days, choose an effective fungicide which also controls septoria. Continue to check for risk updates and monitor crops. Update crop growth stage and date of fungicide applications through the season </t>
   </si>
   <si>
     <t xml:space="preserve">Wenn der Schwellenwert von 20 Stunden Luftfeuchtigkeit nicht überschritten wird, aber andere Krankheiten ebenfalls ein Risiko darstellen und die Kultur in den letzten zehn Tagen nicht behandelt wurde, wählen Sie ein wirksames Fungizid, das auch die Bekämpfung von Septoria abdeckt. 
@@ -1163,7 +1165,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.warning_status_interpretation.4.explanation</t>
   </si>
   <si>
-    <t xml:space="preserve">Based on current observations entered and weather data, the risk of septoria is high.</t>
+    <t xml:space="preserve">Based on weather data and current estimates of crop growth stages and septoria spray dates, the risk of septoria is high. Go to 'Edit parameters' to check and update growth stages and spray dates. This model runs March-June. </t>
   </si>
   <si>
     <t xml:space="preserve">Auf der Grundlage der aktuell eingegebenen Beobachtungen und Wetterdaten besteht ein hohes Septoria-Risiko.</t>
@@ -1190,8 +1192,7 @@
     <t xml:space="preserve">dk.seges.1_1.models.SEPTORIAHU.output.warning_status_interpretation.4.recommended_action</t>
   </si>
   <si>
-    <t xml:space="preserve">If the crop has not been treated against septoria in the last ten days, treat according to need. Choice of fungicides depends on the general disease risk. Apart from effectiveness on septoria the product should also account for other risk factors/diseases.
-This model runs March-June.  Continue to check for risk updates and monitor crops. Update crop growth stage and  date of fungicide applications through the season</t>
+    <t xml:space="preserve">If the crop has not been treated against septoria in the last ten days, treat according to need. Choice of fungicides depends on the general disease risk. Apart from effectiveness on septoria the product should also account for other diseases. Continue to check for risk updates and monitor crops. Update crop growth stage and date of fungicide applications through the season  </t>
   </si>
   <si>
     <t xml:space="preserve">Wurde die Kultur in den letzten zehn Tagen nicht gegen Septoria behandelt, ist eine Behandlung je nach Bedarf durchzuführen. Die Wahl der Fungizide richtet sich nach dem allgemeinen Krankheitsrisiko. Neben der Wirksamkeit gegen Septoria sollte das Produkt auch andere Risikofaktoren/Krankheiten berücksichtigen. 
@@ -1460,19 +1461,19 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1639,24 +1640,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B51" activeCellId="0" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="109.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="106.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="10" style="2" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="90.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="87.94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,65 +1680,58 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" s="3" customFormat="true" ht="93.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>32</v>
       </c>
@@ -1773,15 +1759,15 @@
       <c r="I3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>41</v>
       </c>
@@ -1809,15 +1795,15 @@
       <c r="I4" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>50</v>
       </c>
@@ -1845,15 +1831,15 @@
       <c r="I5" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>59</v>
       </c>
@@ -1881,15 +1867,15 @@
       <c r="I6" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>68</v>
       </c>
@@ -1917,15 +1903,15 @@
       <c r="I7" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>77</v>
       </c>
@@ -1953,15 +1939,15 @@
       <c r="I8" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>86</v>
       </c>
@@ -1989,15 +1975,15 @@
       <c r="I9" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>95</v>
       </c>
@@ -2025,15 +2011,15 @@
       <c r="I10" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>104</v>
       </c>
@@ -2061,15 +2047,15 @@
       <c r="I11" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>113</v>
       </c>
@@ -2097,15 +2083,15 @@
       <c r="I12" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>122</v>
       </c>
@@ -2133,15 +2119,15 @@
       <c r="I13" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>131</v>
       </c>
@@ -2169,15 +2155,15 @@
       <c r="I14" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>140</v>
       </c>
@@ -2205,15 +2191,15 @@
       <c r="I15" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>149</v>
       </c>
@@ -2241,15 +2227,15 @@
       <c r="I16" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>158</v>
       </c>
@@ -2277,15 +2263,15 @@
       <c r="I17" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>167</v>
       </c>
@@ -2313,15 +2299,15 @@
       <c r="I18" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>176</v>
       </c>
@@ -2349,15 +2335,15 @@
       <c r="I19" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>185</v>
       </c>
@@ -2385,15 +2371,15 @@
       <c r="I20" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>193</v>
       </c>
@@ -2421,15 +2407,15 @@
       <c r="I21" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>200</v>
       </c>
@@ -2457,51 +2443,44 @@
       <c r="I22" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-    </row>
-    <row r="23" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>208</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>217</v>
       </c>
@@ -2529,15 +2508,15 @@
       <c r="I24" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>226</v>
       </c>
@@ -2565,15 +2544,15 @@
       <c r="I25" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>235</v>
       </c>
@@ -2601,15 +2580,15 @@
       <c r="I26" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>238</v>
       </c>
@@ -2637,15 +2616,15 @@
       <c r="I27" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>247</v>
       </c>
@@ -2673,15 +2652,15 @@
       <c r="I28" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>248</v>
       </c>
@@ -2709,15 +2688,15 @@
       <c r="I29" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>257</v>
       </c>
@@ -2745,56 +2724,49 @@
       <c r="I30" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-    </row>
-    <row r="31" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
         <v>258</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="G31" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="H31" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>267</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>260</v>
@@ -2817,562 +2789,518 @@
       <c r="I32" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>277</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>286</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C35" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="C36" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="D36" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="F35" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="F36" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="G36" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="H36" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="I36" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="G36" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>305</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G38" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="I38" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="H38" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G39" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="I39" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="H39" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G40" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="I40" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="H40" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-    </row>
-    <row r="41" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="2" t="s">
-        <v>329</v>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+    </row>
+    <row r="41" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>330</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C41" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="D41" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="F41" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="G41" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="H41" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I41" s="3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="B42" s="0" t="s">
         <v>339</v>
       </c>
+      <c r="B42" s="5" t="s">
+        <v>340</v>
+      </c>
       <c r="C42" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-    </row>
-    <row r="43" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
         <v>347</v>
       </c>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>348</v>
+      </c>
       <c r="B43" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="C43" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="D43" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="E43" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="F43" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="G43" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="H43" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-    </row>
-    <row r="44" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="s">
+      <c r="I43" s="3" t="s">
         <v>356</v>
       </c>
+    </row>
+    <row r="44" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>357</v>
+      </c>
       <c r="B44" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="C44" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="F44" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="H44" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-    </row>
-    <row r="45" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="I44" s="3" t="s">
         <v>365</v>
       </c>
+    </row>
+    <row r="45" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>366</v>
+      </c>
       <c r="B45" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="C45" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="E45" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="F45" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="G45" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="H45" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-    </row>
-    <row r="46" s="2" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="I45" s="3" t="s">
         <v>374</v>
       </c>
+    </row>
+    <row r="46" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>375</v>
+      </c>
       <c r="B46" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="C46" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="D46" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="F46" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="G46" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="H46" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I46" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="G47" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="I47" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="H47" s="0" t="s">
-        <v>390</v>
-      </c>
-      <c r="I47" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3393,13 +3321,13 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="65.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="91.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3430,424 +3358,424 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="115.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="246.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+        <v>393</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>394</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+        <v>395</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>396</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+        <v>397</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+        <v>399</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
+        <v>401</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+        <v>402</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+        <v>404</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+        <v>406</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+        <v>409</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+        <v>411</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>412</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+        <v>413</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+        <v>415</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>416</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+        <v>417</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+        <v>418</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>